<commit_message>
Faltan detalles del ejer 6
</commit_message>
<xml_diff>
--- a/Practica6/Plantilla-calculo-hora-trabajador.xlsx
+++ b/Practica6/Plantilla-calculo-hora-trabajador.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unican-my.sharepoint.com/personal/rivasjm_unican_es/Documents/teaching/22-23/2_ingenieria_del_software_ii/6 proyectos/material-estimacion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\UNICAN\3º carrera\2º cuatri\Ingenieria de Software II\IS2_2324\Practica6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_C87741A2305F1A66BA06294065840A12500268A6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{374CE84D-7436-4368-B99E-EA8FE2C062F3}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Coste Hora" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -110,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1]"/>
   </numFmts>
@@ -669,28 +668,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -699,7 +698,7 @@
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="8"/>
@@ -708,7 +707,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -730,7 +729,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -756,7 +755,7 @@
       </c>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="3"/>
@@ -765,7 +764,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -775,13 +774,13 @@
       </c>
       <c r="C6" s="12"/>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -794,67 +793,67 @@
       </c>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="20">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="C9" s="20">
         <v>0</v>
       </c>
       <c r="D9" s="7">
         <f>(B9*12)+C9</f>
-        <v>36000</v>
+        <v>18000</v>
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="7">
         <f>B9*0.3</f>
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7">
         <f>B10*12</f>
-        <v>10800</v>
+        <v>5400</v>
       </c>
       <c r="E10" s="12"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="7">
         <f>B10+B9</f>
-        <v>3900</v>
+        <v>1950</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7">
         <f>D10+D9</f>
-        <v>46800</v>
+        <v>23400</v>
       </c>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -870,7 +869,7 @@
       </c>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -884,26 +883,26 @@
       </c>
       <c r="D17" s="16">
         <f>D11/C17</f>
-        <v>36.5625</v>
+        <v>18.28125</v>
       </c>
       <c r="E17" s="14">
         <f>(D11+B23)/C17</f>
-        <v>38.90625</v>
+        <v>20.625</v>
       </c>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -912,7 +911,7 @@
       </c>
       <c r="C20" s="12"/>
     </row>
-    <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -922,7 +921,7 @@
       </c>
       <c r="C21" s="12"/>
     </row>
-    <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -931,7 +930,7 @@
       </c>
       <c r="C22" s="12"/>
     </row>
-    <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -941,7 +940,7 @@
       </c>
       <c r="C23" s="12"/>
     </row>
-    <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -951,31 +950,31 @@
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B27" s="18">
         <f>(D11+B23)/B6</f>
-        <v>311.25</v>
+        <v>165</v>
       </c>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="11">
         <f>B27*B4</f>
-        <v>6225</v>
+        <v>3300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>